<commit_message>
Title and Olist issue
</commit_message>
<xml_diff>
--- a/translations/csvContent.xlsx
+++ b/translations/csvContent.xlsx
@@ -1627,9 +1627,6 @@
     <t>Lütfen yukarıda ana hatlarıyla belirtildiği gibi müşteri teslimatı için normal süreci izleyin.</t>
   </si>
   <si>
-    <t xml:space="preserve">Olist-element-1-1 </t>
-  </si>
-  <si>
     <t>Olist-element-1-2</t>
   </si>
   <si>
@@ -1640,6 +1637,9 @@
   </si>
   <si>
     <t>Olist-element-1-3</t>
+  </si>
+  <si>
+    <t>Olist-element-1-1</t>
   </si>
 </sst>
 </file>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B11" t="s">
         <v>341</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>

</xml_diff>